<commit_message>
实现early stop world model
</commit_message>
<xml_diff>
--- a/实验记录-DPPO.xlsx
+++ b/实验记录-DPPO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>文件位置</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,65 +46,108 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>PPO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>success rate从0慢慢上升到0.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DPPO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>world model的相对运行次数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>success rate前期比PPO快一些，后面效果没有PPO好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DPPO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reward threshold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>success rate 前期快，后期效果和PPO也差不多</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>world model train epoch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>world model memort size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>success rate 前期更快了，但是增加world model的memory size与train epoches并没有解决后期world model的train accurate下降的问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result/DPPO/DPPO_warm_1000_run_100_reward_threshold_0.5_WM_4_30_5000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存了训练过程中与world model 的对话成功率。DPPO总体的对话成功率为0.85左右</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result/DPPO/DPPO_warm_1000_run_200_wm_2_singlenet_stop_l_0.1_rate_0.9</t>
+  </si>
+  <si>
+    <t>DPPO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是否early stop world model</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result/DPPO/DPPO_warm_1000_run_300_wm_2_singlenet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result/DPPO/DPPO_warm_1000_run_200_wm_2_WM_reward_threshold_0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result/DPPO/DPPO_warm_1000_run_200_wm_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>result/PPO/PPO_warm_1000_run_200</t>
-  </si>
-  <si>
-    <t>PPO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>success rate从0慢慢上升到0.9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>result/DPPO/DPPO_warm_1000_run_200_wm_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stop world model后，准确度不变。似乎只加快了运行速度。需要验证是否在world model K更大时，stop world model 能否提高准确率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result/DPPO/DPPO_warm_1000_run_200_wm_5_singlenet</t>
+  </si>
+  <si>
+    <t>result/DPPO/DPPO_warm_1000_run_200_wm_5_singlenet_stop_l_0.1_rate_0.9</t>
   </si>
   <si>
     <t>DPPO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>world model的相对运行次数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>success rate前期比PPO快一些，后面效果没有PPO好</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DPPO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reward threshold</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>success rate 前期快，后期效果和PPO也差不多</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>world model train epoch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>world model memort size</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>success rate 前期更快了，但是增加world model的memory size与train epoches并没有解决后期world model的train accurate下降的问题</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>result/DPPO/DPPO_warm_1000_run_200_wm_2_WM_reward_threshold_0.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>result/DPPO/DPPO_warm_1000_run_100_reward_threshold_0.5_WM_4_30_5000</t>
+    <t>stop world model后，效果继续上升了。如果不 stop，由于world model效果不好，导致PPO的性能下降</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -112,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +174,12 @@
     <font>
       <sz val="9.8000000000000007"/>
       <color rgb="FFA5C261"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFA9B7C6"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
@@ -157,11 +206,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -444,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -457,12 +509,14 @@
     <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="16.5" customWidth="1"/>
-    <col min="9" max="9" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="18.25" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="10" max="10" width="54.875" customWidth="1"/>
+    <col min="13" max="13" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,27 +530,30 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
       <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
       <c r="C2">
         <v>200</v>
@@ -504,16 +561,16 @@
       <c r="D2">
         <v>1000</v>
       </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>200</v>
@@ -527,16 +584,16 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>200</v>
@@ -556,19 +613,19 @@
       <c r="H4">
         <v>20</v>
       </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D5">
         <v>1000</v>
@@ -585,13 +642,130 @@
       <c r="H5">
         <v>30</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>300</v>
+      </c>
+      <c r="D6">
+        <v>1000</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0.5</v>
+      </c>
+      <c r="G6">
+        <v>3000</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="L6" t="s">
-        <v>8</v>
+      <c r="M6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>200</v>
+      </c>
+      <c r="D7">
+        <v>1000</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0.5</v>
+      </c>
+      <c r="G7">
+        <v>3000</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>1000</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>0.5</v>
+      </c>
+      <c r="G9">
+        <v>3000</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>200</v>
+      </c>
+      <c r="D10">
+        <v>1000</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>0.5</v>
+      </c>
+      <c r="G10">
+        <v>3000</v>
+      </c>
+      <c r="H10">
+        <v>30</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
补做 PPO-6与纠正DPPO-K5-early stop 的实验
</commit_message>
<xml_diff>
--- a/实验记录-DPPO.xlsx
+++ b/实验记录-DPPO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>文件位置</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -150,6 +150,28 @@
   </si>
   <si>
     <t>result/DPPO/DPPO_warm_1000_run_200_wm_5_singlenet_stop_l_0.1_rate_0.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>result/DPPO/DPPO_warm_1000_run_300_simulate_1024_plan_5_stop_l_10_rate_0.9_correct</t>
+  </si>
+  <si>
+    <t>result/PPO/PPO_warm_1000_run_500_simulate_6144</t>
+  </si>
+  <si>
+    <t>DPPO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PPO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个eisode使用的数据量是6倍（6144/1024=6）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>early stop 的正确实验。但是都是在31轮停止的world model</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -157,7 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +207,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF808080"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,7 +236,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -216,6 +244,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -498,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -770,6 +801,55 @@
         <v>29</v>
       </c>
     </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>300</v>
+      </c>
+      <c r="D12">
+        <v>1000</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>0.5</v>
+      </c>
+      <c r="G12">
+        <v>3000</v>
+      </c>
+      <c r="H12">
+        <v>30</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13">
+        <v>500</v>
+      </c>
+      <c r="D13">
+        <v>1000</v>
+      </c>
+      <c r="J13" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>